<commit_message>
Data: expand universities data set
</commit_message>
<xml_diff>
--- a/data/universities.xlsx
+++ b/data/universities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t xml:space="preserve">Institution</t>
   </si>
@@ -74,6 +74,51 @@
   </si>
   <si>
     <t xml:space="preserve">University of Warwick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imperial College London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">King’s College London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Manchester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Bristol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Birmingham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queen Mary University of London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of York</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Nottingham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Dundee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardiff University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Stirling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queen’s University Belfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swansea University</t>
   </si>
 </sst>
 </file>
@@ -88,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -169,15 +215,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.56"/>
@@ -405,6 +451,263 @@
         <v>77</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1907</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>19115</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1064</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1829</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>32895</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>902</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>40250</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>1095.4</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1595</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>25955</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>642.7</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1825</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>35445</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>673.8</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1785</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>20560</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>459.5</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>19470</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>331.4</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1798</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>30798</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>656.5</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1967</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>15915</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>256.4</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1883</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>25898</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>644.8</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1967</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>9548</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>113.3</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1810</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>18438</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>369.2</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1920</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>20620</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Unit 8+9: Various smaller changes, modify universities dataset
</commit_message>
<xml_diff>
--- a/data/universities.xlsx
+++ b/data/universities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t xml:space="preserve">Institution</t>
   </si>
@@ -34,10 +34,16 @@
     <t xml:space="preserve">Students</t>
   </si>
   <si>
+    <t xml:space="preserve">Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Budget</t>
   </si>
   <si>
-    <t xml:space="preserve">Rank</t>
+    <t xml:space="preserve">Russell</t>
   </si>
   <si>
     <t xml:space="preserve">University of Glasgow</t>
@@ -215,20 +221,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,13 +258,19 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1451</v>
@@ -265,18 +279,24 @@
         <v>30805</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>2942</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>4003</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>626.5</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>92</v>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1583</v>
@@ -285,18 +305,24 @@
         <v>34275</v>
       </c>
       <c r="E3" s="0" t="n">
+        <v>4589</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>6107</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>1102</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>30</v>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1413</v>
@@ -305,18 +331,24 @@
         <v>8984</v>
       </c>
       <c r="E4" s="0" t="n">
+        <v>1137</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1576</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>251.2</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>201</v>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1495</v>
@@ -325,18 +357,24 @@
         <v>14775</v>
       </c>
       <c r="E5" s="0" t="n">
+        <v>1086</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1489</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>219.5</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>178</v>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1964</v>
@@ -344,19 +382,22 @@
       <c r="D6" s="0" t="n">
         <v>22640</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="F6" s="0" t="n">
+        <v>3200</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>304.4</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>401</v>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1895</v>
@@ -365,18 +406,24 @@
         <v>11850</v>
       </c>
       <c r="E7" s="0" t="n">
+        <v>1725</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2515</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>415.1</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>27</v>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1826</v>
@@ -385,18 +432,24 @@
         <v>41180</v>
       </c>
       <c r="E8" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>5375</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>1451.1</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>16</v>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1209</v>
@@ -405,18 +458,24 @@
         <v>23247</v>
       </c>
       <c r="E9" s="0" t="n">
+        <v>7913</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>3615</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>2192</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>6</v>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1096</v>
@@ -425,18 +484,21 @@
         <v>24515</v>
       </c>
       <c r="E10" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>2450</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1965</v>
@@ -445,18 +507,24 @@
         <v>27278</v>
       </c>
       <c r="E11" s="0" t="n">
+        <v>2610</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>4033</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>688.6</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>77</v>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1907</v>
@@ -465,18 +533,24 @@
         <v>19115</v>
       </c>
       <c r="E12" s="0" t="n">
+        <v>4390</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>4075</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>1064</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>11</v>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1829</v>
@@ -485,18 +559,24 @@
         <v>32895</v>
       </c>
       <c r="E13" s="0" t="n">
+        <v>5220</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>3485</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>902</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>35</v>
+      <c r="H13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>2004</v>
@@ -505,18 +585,21 @@
         <v>40250</v>
       </c>
       <c r="E14" s="0" t="n">
+        <v>3849</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>1095.4</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>51</v>
+      <c r="H14" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1595</v>
@@ -525,18 +608,24 @@
         <v>25955</v>
       </c>
       <c r="E15" s="0" t="n">
+        <v>3285</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>6199</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>642.7</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>91</v>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1825</v>
@@ -545,18 +634,21 @@
         <v>35445</v>
       </c>
       <c r="E16" s="0" t="n">
+        <v>4020</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>673.8</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>107</v>
+      <c r="H16" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1785</v>
@@ -565,18 +657,24 @@
         <v>20560</v>
       </c>
       <c r="E17" s="0" t="n">
+        <v>3235</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>4620</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>459.5</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>110</v>
+      <c r="H17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1963</v>
@@ -585,18 +683,24 @@
         <v>19470</v>
       </c>
       <c r="E18" s="0" t="n">
+        <v>1935</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3091</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>331.4</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>133</v>
+      <c r="H18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1798</v>
@@ -605,18 +709,21 @@
         <v>30798</v>
       </c>
       <c r="E19" s="0" t="n">
+        <v>3495</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>656.5</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>158</v>
+      <c r="H19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1967</v>
@@ -625,18 +732,24 @@
         <v>15915</v>
       </c>
       <c r="E20" s="0" t="n">
+        <v>1410</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1805</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>256.4</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>201</v>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1883</v>
@@ -645,18 +758,24 @@
         <v>25898</v>
       </c>
       <c r="E21" s="0" t="n">
+        <v>3330</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5739</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>644.8</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <v>191</v>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1967</v>
@@ -664,19 +783,22 @@
       <c r="D22" s="0" t="n">
         <v>9548</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="F22" s="0" t="n">
+        <v>1872</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>113.3</v>
       </c>
-      <c r="F22" s="0" t="n">
-        <v>301</v>
+      <c r="H22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1810</v>
@@ -685,18 +807,24 @@
         <v>18438</v>
       </c>
       <c r="E23" s="0" t="n">
+        <v>2414</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1489</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>369.2</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>200</v>
+      <c r="H23" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1920</v>
@@ -705,7 +833,10 @@
         <v>20620</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>251</v>
+        <v>3290</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>